<commit_message>
improve excel for lab3
</commit_message>
<xml_diff>
--- a/Coursework Reports/3rd assignment/xlsx3.xlsx
+++ b/Coursework Reports/3rd assignment/xlsx3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99DA2F3-865D-4D53-9E1B-F08A6D02B3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC59B7E-2D58-4442-B640-7A902B096B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5749,16 +5749,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19048,7 +19048,7 @@
   <dimension ref="A1:S702"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>